<commit_message>
feat: adding new database, small refactor and adding PP proposal
</commit_message>
<xml_diff>
--- a/tables/indicadores_percentis_renda_extendido.xlsx
+++ b/tables/indicadores_percentis_renda_extendido.xlsx
@@ -422,25 +422,25 @@
         <v>1490.19247005712</v>
       </c>
       <c r="D2">
-        <v>30054.906423647</v>
+        <v>31642.2046022216</v>
       </c>
       <c r="E2">
         <v>896.60399247551</v>
       </c>
       <c r="F2">
-        <v>28564.71395358988</v>
+        <v>30152.01213216448</v>
       </c>
       <c r="G2">
         <v>2.51048078987052</v>
       </c>
       <c r="H2">
-        <v>20.16847288356985</v>
+        <v>21.2336360825986</v>
       </c>
       <c r="I2">
-        <v>419847.0506074061</v>
+        <v>474634.3916791933</v>
       </c>
       <c r="J2">
-        <v>281.7401503789058</v>
+        <v>318.5054288061194</v>
       </c>
     </row>
     <row r="3">
@@ -456,25 +456,25 @@
         <v>1490.19247005712</v>
       </c>
       <c r="D3">
-        <v>30054.906423647</v>
+        <v>31642.2046022216</v>
       </c>
       <c r="E3">
         <v>896.60399247551</v>
       </c>
       <c r="F3">
-        <v>28564.71395358988</v>
+        <v>30152.01213216448</v>
       </c>
       <c r="G3">
         <v>2.51048078987052</v>
       </c>
       <c r="H3">
-        <v>20.16847288356985</v>
+        <v>21.2336360825986</v>
       </c>
       <c r="I3">
-        <v>400949.3352854665</v>
+        <v>471032.0562202815</v>
       </c>
       <c r="J3">
-        <v>269.0587580744505</v>
+        <v>316.088066263163</v>
       </c>
     </row>
     <row r="4">
@@ -490,25 +490,25 @@
         <v>1490.19247005712</v>
       </c>
       <c r="D4">
-        <v>29963.6482688337</v>
+        <v>31642.2046022216</v>
       </c>
       <c r="E4">
         <v>896.60399247551</v>
       </c>
       <c r="F4">
-        <v>28473.45579877658</v>
+        <v>30152.01213216448</v>
       </c>
       <c r="G4">
         <v>2.51048078987052</v>
       </c>
       <c r="H4">
-        <v>20.10723371034426</v>
+        <v>21.2336360825986</v>
       </c>
       <c r="I4">
-        <v>393975.7643331102</v>
+        <v>471032.0562202815</v>
       </c>
       <c r="J4">
-        <v>264.3791136040359</v>
+        <v>316.088066263163</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: code updates to incorporate new tax rules
</commit_message>
<xml_diff>
--- a/tables/indicadores_percentis_renda_extendido.xlsx
+++ b/tables/indicadores_percentis_renda_extendido.xlsx
@@ -422,25 +422,25 @@
         <v>1490.19247005712</v>
       </c>
       <c r="D2">
-        <v>31642.2046022216</v>
+        <v>30332.8980555797</v>
       </c>
       <c r="E2">
         <v>896.60399247551</v>
       </c>
       <c r="F2">
-        <v>30152.01213216448</v>
+        <v>28842.70558552258</v>
       </c>
       <c r="G2">
         <v>2.51048078987052</v>
       </c>
       <c r="H2">
-        <v>21.2336360825986</v>
+        <v>20.35502035144294</v>
       </c>
       <c r="I2">
-        <v>474634.3916791933</v>
+        <v>416326.5901685993</v>
       </c>
       <c r="J2">
-        <v>318.5054288061194</v>
+        <v>279.3777304166899</v>
       </c>
     </row>
     <row r="3">
@@ -456,25 +456,25 @@
         <v>1490.19247005712</v>
       </c>
       <c r="D3">
-        <v>31642.2046022216</v>
+        <v>30332.8980555797</v>
       </c>
       <c r="E3">
         <v>896.60399247551</v>
       </c>
       <c r="F3">
-        <v>30152.01213216448</v>
+        <v>28842.70558552258</v>
       </c>
       <c r="G3">
         <v>2.51048078987052</v>
       </c>
       <c r="H3">
-        <v>21.2336360825986</v>
+        <v>20.35502035144294</v>
       </c>
       <c r="I3">
-        <v>471032.0562202815</v>
+        <v>401008.5384240549</v>
       </c>
       <c r="J3">
-        <v>316.088066263163</v>
+        <v>269.098486592597</v>
       </c>
     </row>
     <row r="4">
@@ -490,25 +490,25 @@
         <v>1490.19247005712</v>
       </c>
       <c r="D4">
-        <v>31642.2046022216</v>
+        <v>30259.6043376406</v>
       </c>
       <c r="E4">
         <v>896.60399247551</v>
       </c>
       <c r="F4">
-        <v>30152.01213216448</v>
+        <v>28769.41186758348</v>
       </c>
       <c r="G4">
         <v>2.51048078987052</v>
       </c>
       <c r="H4">
-        <v>21.2336360825986</v>
+        <v>20.30583629004697</v>
       </c>
       <c r="I4">
-        <v>471032.0562202815</v>
+        <v>398275.8910160765</v>
       </c>
       <c r="J4">
-        <v>316.088066263163</v>
+        <v>267.2647319180255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adding inflation function
</commit_message>
<xml_diff>
--- a/tables/indicadores_percentis_renda_extendido.xlsx
+++ b/tables/indicadores_percentis_renda_extendido.xlsx
@@ -416,31 +416,31 @@
         </is>
       </c>
       <c r="B2">
-        <v>593.5884775816101</v>
+        <v>688.562633994668</v>
       </c>
       <c r="C2">
-        <v>1490.19247005712</v>
+        <v>1728.62326526626</v>
       </c>
       <c r="D2">
-        <v>30332.8980555797</v>
+        <v>35186.1617444724</v>
       </c>
       <c r="E2">
-        <v>896.60399247551</v>
+        <v>1040.060631271592</v>
       </c>
       <c r="F2">
-        <v>28842.70558552258</v>
+        <v>33457.53847920614</v>
       </c>
       <c r="G2">
         <v>2.51048078987052</v>
       </c>
       <c r="H2">
-        <v>20.35502035144294</v>
+        <v>20.3550203514429</v>
       </c>
       <c r="I2">
-        <v>416326.5901685993</v>
+        <v>488332.0497994241</v>
       </c>
       <c r="J2">
-        <v>279.3777304166899</v>
+        <v>282.497672923664</v>
       </c>
     </row>
     <row r="3">
@@ -450,31 +450,31 @@
         </is>
       </c>
       <c r="B3">
-        <v>593.5884775816101</v>
+        <v>688.562633994668</v>
       </c>
       <c r="C3">
-        <v>1490.19247005712</v>
+        <v>1728.62326526626</v>
       </c>
       <c r="D3">
-        <v>30332.8980555797</v>
+        <v>35186.1617444724</v>
       </c>
       <c r="E3">
-        <v>896.60399247551</v>
+        <v>1040.060631271592</v>
       </c>
       <c r="F3">
-        <v>28842.70558552258</v>
+        <v>33457.53847920614</v>
       </c>
       <c r="G3">
         <v>2.51048078987052</v>
       </c>
       <c r="H3">
-        <v>20.35502035144294</v>
+        <v>20.3550203514429</v>
       </c>
       <c r="I3">
-        <v>401008.5384240549</v>
+        <v>465216.8427860898</v>
       </c>
       <c r="J3">
-        <v>269.098486592597</v>
+        <v>269.1256401170976</v>
       </c>
     </row>
     <row r="4">
@@ -484,31 +484,31 @@
         </is>
       </c>
       <c r="B4">
-        <v>593.5884775816101</v>
+        <v>688.562633994668</v>
       </c>
       <c r="C4">
-        <v>1490.19247005712</v>
+        <v>1728.62326526626</v>
       </c>
       <c r="D4">
-        <v>30259.6043376406</v>
+        <v>35121.9072044382</v>
       </c>
       <c r="E4">
-        <v>896.60399247551</v>
+        <v>1040.060631271592</v>
       </c>
       <c r="F4">
-        <v>28769.41186758348</v>
+        <v>33393.28393917194</v>
       </c>
       <c r="G4">
         <v>2.51048078987052</v>
       </c>
       <c r="H4">
-        <v>20.30583629004697</v>
+        <v>20.31784941817752</v>
       </c>
       <c r="I4">
-        <v>398275.8910160765</v>
+        <v>462368.2441667155</v>
       </c>
       <c r="J4">
-        <v>267.2647319180255</v>
+        <v>267.4777399200959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: adding Arthen's implementation for reduction in dividends + small adjustments
</commit_message>
<xml_diff>
--- a/tables/indicadores_percentis_renda_extendido.xlsx
+++ b/tables/indicadores_percentis_renda_extendido.xlsx
@@ -422,25 +422,25 @@
         <v>1728.62326526626</v>
       </c>
       <c r="D2">
-        <v>35186.1617444724</v>
+        <v>34958.9187444724</v>
       </c>
       <c r="E2">
         <v>1040.060631271592</v>
       </c>
       <c r="F2">
-        <v>33457.53847920614</v>
+        <v>33230.29547920614</v>
       </c>
       <c r="G2">
         <v>2.51048078987052</v>
       </c>
       <c r="H2">
-        <v>20.3550203514429</v>
+        <v>20.22356140109434</v>
       </c>
       <c r="I2">
-        <v>488332.0497994241</v>
+        <v>488104.8067994241</v>
       </c>
       <c r="J2">
-        <v>282.497672923664</v>
+        <v>282.3662139733155</v>
       </c>
     </row>
     <row r="3">
@@ -456,25 +456,25 @@
         <v>1728.62326526626</v>
       </c>
       <c r="D3">
-        <v>35186.1617444724</v>
+        <v>34958.9187444724</v>
       </c>
       <c r="E3">
         <v>1040.060631271592</v>
       </c>
       <c r="F3">
-        <v>33457.53847920614</v>
+        <v>33230.29547920614</v>
       </c>
       <c r="G3">
         <v>2.51048078987052</v>
       </c>
       <c r="H3">
-        <v>20.3550203514429</v>
+        <v>20.22356140109434</v>
       </c>
       <c r="I3">
-        <v>465216.8427860898</v>
+        <v>465205.9881384756</v>
       </c>
       <c r="J3">
-        <v>269.1256401170976</v>
+        <v>269.1193607571976</v>
       </c>
     </row>
     <row r="4">
@@ -490,25 +490,25 @@
         <v>1728.62326526626</v>
       </c>
       <c r="D4">
-        <v>35121.9072044382</v>
+        <v>34853.059284889</v>
       </c>
       <c r="E4">
         <v>1040.060631271592</v>
       </c>
       <c r="F4">
-        <v>33393.28393917194</v>
+        <v>33124.43601962274</v>
       </c>
       <c r="G4">
         <v>2.51048078987052</v>
       </c>
       <c r="H4">
-        <v>20.31784941817752</v>
+        <v>20.16232222786877</v>
       </c>
       <c r="I4">
-        <v>462368.2441667155</v>
+        <v>458592.727236731</v>
       </c>
       <c r="J4">
-        <v>267.4777399200959</v>
+        <v>265.2936220698696</v>
       </c>
     </row>
   </sheetData>

</xml_diff>